<commit_message>
Add/Update nuget packages to solution projects, Add API documentation
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/SalesData.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/SalesData.xlsx
@@ -252,50 +252,50 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0"/>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" xfId="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" xfId="1" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="3" applyFill="1" xfId="2">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="3" applyFill="1" xfId="2" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="3" applyFill="1" xfId="3">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="2" applyFont="1" fillId="3" applyFill="1" xfId="3" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" xfId="4">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" xfId="4" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="1" applyBorder="1" xfId="5">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="1" applyBorder="1" xfId="5" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="6">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="6" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="7">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="7" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="8">
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="8" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="9">
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="9" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="10">
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="10" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="11">
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="11" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="3" applyBorder="1" xfId="12">
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="3" applyBorder="1" xfId="12" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="3" applyBorder="1" xfId="13">
+    <xf numFmtId="165" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="3" applyBorder="1" xfId="13" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="6">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" xfId="6" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="7">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="3" applyFont="1" fillId="5" applyFill="1" borderId="2" applyBorder="1" xfId="7" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>

</xml_diff>